<commit_message>
≡ƒôè Weekly data update
</commit_message>
<xml_diff>
--- a/Weekly Expenditure.xlsx
+++ b/Weekly Expenditure.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://osram-my.sharepoint.com/personal/azhar_arkam_ams_com/Documents/Desktop/Daily Files/Inventory Y25 for SLK + LF/Tong Inventory List Weekly/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://osram-my.sharepoint.com/personal/azhar_arkam_ams_com/Documents/amoa/DropBox III/Desktop/EongsRequest/ploty_Dashboard/Weeklydashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{82A9AC4F-F022-4B3A-85D3-C409B9F30705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D45156C-7B0E-49A7-A6AE-53B410A48E50}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="8_{82A9AC4F-F022-4B3A-85D3-C409B9F30705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BE3CAAD-C8F7-4066-A6A9-249693233928}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CAB9E47C-89B0-4422-B529-4EB28642A4AC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="101">
   <si>
     <t>WorkWeek</t>
   </si>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t>SAP</t>
+  </si>
+  <si>
+    <t>Wk28</t>
   </si>
 </sst>
 </file>
@@ -722,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45189669-8C26-4695-95A4-FB3154B5D562}">
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2013,6 +2016,110 @@
         <v>1680</v>
       </c>
     </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G50" s="2">
+        <v>45841</v>
+      </c>
+      <c r="H50" s="1">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G51" s="2">
+        <v>45841</v>
+      </c>
+      <c r="H51" s="1">
+        <v>1075.28</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" s="1">
+        <v>11155497</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G52" s="2">
+        <v>45841</v>
+      </c>
+      <c r="H52" s="1">
+        <v>561.6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G53" s="2">
+        <v>45842</v>
+      </c>
+      <c r="H53" s="1">
+        <v>1680</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>